<commit_message>
Glossary for website + automatic table generation
</commit_message>
<xml_diff>
--- a/RRDS_extraction/PGA argument descriptions for Paul.xlsx
+++ b/RRDS_extraction/PGA argument descriptions for Paul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmmcgilchrist\Downloads\MMM\Ontologies\PGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenLHSRepo\DASH-Onto\RRDS_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF4FB6-7D9B-4EE5-A416-6575C7F38398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507B77F2-CF54-47F4-B9DA-838C93CD4539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F766D281-F559-4AFB-8FE8-013C565CFBB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F766D281-F559-4AFB-8FE8-013C565CFBB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -3194,9 +3194,6 @@
     <t>luw_DASH_Oversight</t>
   </si>
   <si>
-    <t>usedLocations</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -3870,6 +3867,9 @@
   </si>
   <si>
     <t>PLAN</t>
+  </si>
+  <si>
+    <t>OUT: usedLocations</t>
   </si>
 </sst>
 </file>
@@ -3990,7 +3990,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4288,16 +4288,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0C1811-C989-4860-AA56-271D8E680A75}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="98.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="280.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="280.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4309,21 +4309,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A152F43-BDD9-4621-94A4-EA0C50B56FAB}">
   <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.08984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="65.26953125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="65.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
         <v>26</v>
@@ -4452,7 +4452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>22</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>39</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
         <v>41</v>
@@ -4547,7 +4547,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
         <v>42</v>
@@ -4560,7 +4560,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>43</v>
@@ -4573,7 +4573,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>53</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>54</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
         <v>55</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>60</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
         <v>62</v>
@@ -4661,7 +4661,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -4670,7 +4670,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D32" s="5" t="s">
         <v>22</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
         <v>22</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>75</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>78</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>22</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>80</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D39" s="5" t="s">
         <v>22</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
         <v>22</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>90</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>93</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
         <v>22</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>50</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>97</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
         <v>98</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D48" s="5" t="s">
         <v>99</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D49" s="5" t="s">
         <v>100</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>105</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>22</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>109</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>62</v>
@@ -4946,7 +4946,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>112</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>114</v>
       </c>
@@ -4965,7 +4965,7 @@
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>116</v>
       </c>
@@ -4976,7 +4976,7 @@
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>117</v>
       </c>
@@ -4987,7 +4987,7 @@
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>119</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D62" s="5" t="s">
         <v>22</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>121</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D64" s="5" t="s">
         <v>22</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>123</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D66" s="5" t="s">
         <v>22</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>125</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
         <v>22</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>127</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
         <v>22</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>129</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D72" s="5" t="s">
         <v>22</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>131</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>146</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
         <v>22</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>149</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
         <v>22</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>152</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>155</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>22</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>157</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>22</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>159</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
         <v>22</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>161</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
         <v>22</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D90" s="5" t="s">
         <v>22</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>165</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>177</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
         <v>22</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>179</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>184</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D99" s="5" t="s">
         <v>22</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>185</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D101" s="5" t="s">
         <v>22</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>186</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D103" s="5" t="s">
         <v>22</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>188</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>22</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
         <v>197</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>199</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
         <v>22</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
         <v>50</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D111" s="5" t="s">
         <v>97</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D112" s="5" t="s">
         <v>98</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D113" s="5" t="s">
         <v>205</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>207</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>100</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>210</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D118" s="5" t="s">
         <v>22</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
         <v>212</v>
       </c>
@@ -5633,7 +5633,7 @@
       <c r="D120" s="11"/>
       <c r="E120" s="10"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>213</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
         <v>214</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="D122" s="11"/>
       <c r="E122" s="10"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="s">
         <v>215</v>
       </c>
@@ -5663,7 +5663,7 @@
       <c r="D123" s="11"/>
       <c r="E123" s="10"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
         <v>216</v>
       </c>
@@ -5674,7 +5674,7 @@
       <c r="D124" s="11"/>
       <c r="E124" s="10"/>
     </row>
-    <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -5683,7 +5683,7 @@
       </c>
       <c r="E126" s="6"/>
     </row>
-    <row r="128" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>219</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
         <v>220</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D130" s="5" t="s">
         <v>22</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>226</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="10" t="s">
         <v>228</v>
@@ -5745,7 +5745,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>230</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
         <v>232</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>22</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>234</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
         <v>243</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>22</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>237</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="10" t="s">
         <v>239</v>
@@ -5845,7 +5845,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="10" t="s">
         <v>240</v>
@@ -5858,7 +5858,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>244</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
         <v>245</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D149" s="5" t="s">
         <v>22</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
         <v>248</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
       <c r="B152" s="10" t="s">
         <v>249</v>
@@ -5922,7 +5922,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>251</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
         <v>252</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D156" s="5" t="s">
         <v>22</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
         <v>255</v>
       </c>
@@ -5971,7 +5971,7 @@
       <c r="D157" s="11"/>
       <c r="E157" s="10"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
       <c r="B158" s="10" t="s">
         <v>256</v>
@@ -5984,7 +5984,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>258</v>
       </c>
@@ -5998,61 +5998,61 @@
         <v>19</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="D161" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D162" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D163" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E163" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="D163" s="5" t="s">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D164" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E164" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D164" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E164" s="3" t="s">
+    <row r="165" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B165" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E165" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B165" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E165" s="3" t="s">
+    <row r="167" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="10" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A167" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="B167" s="10" t="s">
         <v>221</v>
@@ -6062,25 +6062,25 @@
       </c>
       <c r="D167" s="11"/>
       <c r="E167" s="10" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="10"/>
       <c r="B168" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D168" s="11"/>
       <c r="E168" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B170" s="10" t="s">
         <v>231</v>
@@ -6090,51 +6090,51 @@
       </c>
       <c r="D170" s="11"/>
       <c r="E170" s="10" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="B171" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D171" s="11"/>
       <c r="E171" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B173" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="C173" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E173" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C173" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D173" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E175" s="6"/>
     </row>
-    <row r="177" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B177" s="10" t="s">
         <v>221</v>
@@ -6144,7 +6144,7 @@
       </c>
       <c r="D177" s="11"/>
       <c r="E177" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>